<commit_message>
updated the API for negative scenario
</commit_message>
<xml_diff>
--- a/ConfigurationFolder/testscript/TestData.xlsx
+++ b/ConfigurationFolder/testscript/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="54">
   <si>
     <t>End</t>
   </si>
@@ -163,12 +163,45 @@
   <si>
     <t>Fire TV Cube112</t>
   </si>
+  <si>
+    <t>petid</t>
+  </si>
+  <si>
+    <t>status code</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>48956</t>
+  </si>
+  <si>
+    <t>404</t>
+  </si>
+  <si>
+    <t>Pet not found</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>TC_EC_0005</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,13 +214,6 @@
       <color indexed="12"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="4"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -210,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -221,9 +247,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -533,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B13" sqref="B13:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -560,38 +583,38 @@
     <col min="21" max="21" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:7">
       <c r="B2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4">
-      <c r="B3" s="5" t="s">
+    <row r="3" spans="1:7">
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
@@ -602,94 +625,143 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" customHeight="1">
+    <row r="6" spans="1:7" ht="15" customHeight="1">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1">
+    <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="A7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="6"/>
-    </row>
-    <row r="8" spans="1:4" ht="15" customHeight="1">
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1">
       <c r="A8" t="s">
         <v>5</v>
       </c>
       <c r="B8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" customHeight="1">
+    <row r="9" spans="1:7" ht="15" customHeight="1">
       <c r="A9" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="6"/>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1">
       <c r="A10" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1">
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s">
+        <v>50</v>
+      </c>
+      <c r="F11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D13" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="B11" s="1" t="s">
+    <row r="14" spans="1:7">
+      <c r="B14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="B12" s="5" t="s">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="B15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D15" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
-      <c r="B13" s="1" t="s">
+    <row r="16" spans="1:7">
+      <c r="B16" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D16" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
-      <c r="A14" t="s">
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
-      <c r="A15" t="s">
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>